<commit_message>
updated 25th of Aug
</commit_message>
<xml_diff>
--- a/dist/data/sites.xlsx
+++ b/dist/data/sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bautek-hompage\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9288C5FA-9D4D-4677-BC48-1727AAD4C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407089FC-4AA6-4CEE-84E2-3AF60F3A2AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90DA7668-941B-45E8-8F84-C63A56E1DFC5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="113">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -408,6 +408,22 @@
   </si>
   <si>
     <t>포스코오티에르</t>
+  </si>
+  <si>
+    <t>지역</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>준공년도</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수도권</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024년</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1052,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F26BF3-C1EC-4B70-A86E-5EB058D5B44F}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1064,10 +1080,12 @@
     <col min="3" max="3" width="25.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="43.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="30" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1084,13 +1102,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1106,14 +1130,20 @@
       <c r="E2" s="3">
         <v>86</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="6">
         <v>35.859352999999999</v>
       </c>
-      <c r="G2" s="7">
+      <c r="I2" s="7">
         <v>128.55867799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1127,14 +1157,20 @@
       <c r="E3" s="8">
         <v>2633</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="11">
         <v>37.383980000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="I3" s="12">
         <v>126.979345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1150,14 +1186,20 @@
       <c r="E4" s="8">
         <v>3804</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="11">
         <v>37.482711999999999</v>
       </c>
-      <c r="G4" s="12">
+      <c r="I4" s="12">
         <v>126.86873199999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1173,14 +1215,20 @@
       <c r="E5" s="8">
         <v>1490</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="11">
         <v>37.485453</v>
       </c>
-      <c r="G5" s="12">
+      <c r="I5" s="12">
         <v>126.868335</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
@@ -1196,14 +1244,20 @@
       <c r="E6" s="8">
         <v>1758</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="11">
         <v>35.855117999999997</v>
       </c>
-      <c r="G6" s="12">
+      <c r="I6" s="12">
         <v>128.59344100000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
@@ -1217,14 +1271,20 @@
       <c r="E7" s="8">
         <v>2180</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="11">
         <v>37.390790000000003</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>126.983385</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
@@ -1240,14 +1300,20 @@
       <c r="E8" s="8">
         <v>992</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="11">
         <v>35.226903</v>
       </c>
-      <c r="G8" s="12">
+      <c r="I8" s="12">
         <v>128.89164099999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
@@ -1263,14 +1329,20 @@
       <c r="E9" s="8">
         <v>707</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="11">
         <v>35.582918999999997</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>126.844069</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -1287,14 +1359,20 @@
         <f>739+849</f>
         <v>1588</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="11">
         <v>36.768129999999999</v>
       </c>
-      <c r="G10" s="12">
+      <c r="I10" s="12">
         <v>127.002917</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
@@ -1310,14 +1388,20 @@
       <c r="E11" s="8">
         <v>677</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="11">
         <v>34.930737999999998</v>
       </c>
-      <c r="G11" s="12">
+      <c r="I11" s="12">
         <v>128.08571699999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
@@ -1333,14 +1417,20 @@
       <c r="E12" s="8">
         <v>625</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="11">
         <v>37.598376999999999</v>
       </c>
-      <c r="G12" s="12">
+      <c r="I12" s="12">
         <v>126.697428</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>39</v>
       </c>
@@ -1356,14 +1446,20 @@
       <c r="E13" s="8">
         <v>535</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="11">
         <v>37.542867999999999</v>
       </c>
-      <c r="G13" s="12">
+      <c r="I13" s="12">
         <v>127.125702</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1379,14 +1475,20 @@
       <c r="E14" s="8">
         <v>322</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="11">
         <v>35.876660999999999</v>
       </c>
-      <c r="G14" s="12">
+      <c r="I14" s="12">
         <v>128.62753699999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>43</v>
       </c>
@@ -1402,14 +1504,20 @@
       <c r="E15" s="20">
         <v>1458</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="11">
         <v>37.596037000000003</v>
       </c>
-      <c r="G15" s="12">
+      <c r="I15" s="12">
         <v>126.71882100000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
@@ -1425,14 +1533,20 @@
       <c r="E16" s="8">
         <v>262</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="11">
         <v>37.598340999999998</v>
       </c>
-      <c r="G16" s="12">
+      <c r="I16" s="12">
         <v>126.909711</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
@@ -1448,14 +1562,20 @@
       <c r="E17" s="8">
         <v>558</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="11">
         <v>37.293013000000002</v>
       </c>
-      <c r="G17" s="12">
+      <c r="I17" s="12">
         <v>127.450344</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>49</v>
       </c>
@@ -1471,14 +1591,20 @@
       <c r="E18" s="21">
         <v>1626</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="11">
         <v>36.792288999999997</v>
       </c>
-      <c r="G18" s="12">
+      <c r="I18" s="12">
         <v>127.056669</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>51</v>
       </c>
@@ -1494,14 +1620,20 @@
       <c r="E19" s="8">
         <v>343</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="11">
         <v>34.868617</v>
       </c>
-      <c r="G19" s="12">
+      <c r="I19" s="12">
         <v>128.72651500000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>55</v>
       </c>
@@ -1517,14 +1649,20 @@
       <c r="E20" s="8">
         <v>415</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="11">
         <v>35.258766999999999</v>
       </c>
-      <c r="G20" s="12">
+      <c r="I20" s="12">
         <v>129.09251599999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>57</v>
       </c>
@@ -1540,14 +1678,20 @@
       <c r="E21" s="8">
         <v>577</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="11">
         <v>37.559583000000003</v>
       </c>
-      <c r="G21" s="12">
+      <c r="I21" s="12">
         <v>126.81936399999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>61</v>
       </c>
@@ -1563,14 +1707,20 @@
       <c r="E22" s="8">
         <v>212</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="11">
         <v>36.052664999999998</v>
       </c>
-      <c r="G22" s="12">
+      <c r="I22" s="12">
         <v>129.37558300000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>63</v>
       </c>
@@ -1586,14 +1736,20 @@
       <c r="E23" s="8">
         <v>458</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="11">
         <v>37.374136</v>
       </c>
-      <c r="G23" s="12">
+      <c r="I23" s="12">
         <v>126.95327399999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>67</v>
       </c>
@@ -1609,14 +1765,20 @@
       <c r="E24" s="8">
         <v>949</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="11">
         <v>36.645383000000002</v>
       </c>
-      <c r="G24" s="12">
+      <c r="I24" s="12">
         <v>126.683842</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>69</v>
       </c>
@@ -1632,14 +1794,20 @@
       <c r="E25" s="8">
         <v>970</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="15">
         <v>37.316023999999999</v>
       </c>
-      <c r="G25" s="12">
+      <c r="I25" s="12">
         <v>127.951711</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>71</v>
       </c>
@@ -1655,14 +1823,20 @@
       <c r="E26" s="8">
         <v>438</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="15">
         <v>35.837752999999999</v>
       </c>
-      <c r="G26" s="16">
+      <c r="I26" s="16">
         <v>128.53311400000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>73</v>
       </c>
@@ -1678,14 +1852,20 @@
       <c r="E27" s="8">
         <v>732</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="15">
         <v>37.601111000000003</v>
       </c>
-      <c r="G27" s="12">
+      <c r="I27" s="12">
         <v>126.673773</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>75</v>
       </c>
@@ -1701,14 +1881,20 @@
       <c r="E28" s="13">
         <v>800</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="11">
         <v>35.983002999999997</v>
       </c>
-      <c r="G28" s="12">
+      <c r="I28" s="12">
         <v>126.74664300000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>77</v>
       </c>
@@ -1724,14 +1910,20 @@
       <c r="E29" s="13">
         <v>709</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="11">
         <v>37.610427000000001</v>
       </c>
-      <c r="G29" s="12">
+      <c r="I29" s="12">
         <v>126.682586</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>79</v>
       </c>
@@ -1747,14 +1939,20 @@
       <c r="E30" s="13">
         <v>464</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="11">
         <v>37.192450000000001</v>
       </c>
-      <c r="G30" s="12">
+      <c r="I30" s="12">
         <v>127.090754</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>83</v>
       </c>
@@ -1770,14 +1968,20 @@
       <c r="E31" s="13">
         <v>548</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" s="11">
         <v>37.378968999999998</v>
       </c>
-      <c r="G31" s="12">
+      <c r="I31" s="12">
         <v>126.680836</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>85</v>
       </c>
@@ -1793,14 +1997,20 @@
       <c r="E32" s="13">
         <v>1305</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="11">
         <v>37.572637</v>
       </c>
-      <c r="G32" s="12">
+      <c r="I32" s="12">
         <v>127.16999</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
         <v>89</v>
       </c>
@@ -1816,14 +2026,20 @@
       <c r="E33" s="27">
         <v>1305</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="28">
         <v>37.572637</v>
       </c>
-      <c r="G33" s="29">
+      <c r="I33" s="29">
         <v>127.16999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>93</v>
       </c>
@@ -1839,14 +2055,20 @@
       <c r="E34" s="13">
         <v>731</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="11">
         <v>35.581713000000001</v>
       </c>
-      <c r="G34" s="12">
+      <c r="I34" s="12">
         <v>129.26778100000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>97</v>
       </c>
@@ -1862,14 +2084,20 @@
       <c r="E35" s="23">
         <v>311</v>
       </c>
-      <c r="F35" s="24">
+      <c r="F35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="24">
         <v>35.548447000000003</v>
       </c>
-      <c r="G35" s="25">
+      <c r="I35" s="25">
         <v>129.322126</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>101</v>
       </c>
@@ -1885,14 +2113,20 @@
       <c r="E36" s="32">
         <v>2091</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" s="33">
         <v>37.500635000000003</v>
       </c>
-      <c r="G36" s="33">
+      <c r="I36" s="33">
         <v>126.98910100000001</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>105</v>
       </c>
@@ -1908,10 +2142,16 @@
       <c r="E37" s="32">
         <v>182</v>
       </c>
-      <c r="F37" s="33">
+      <c r="F37" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" s="33">
         <v>37.520178000000001</v>
       </c>
-      <c r="G37" s="34">
+      <c r="I37" s="34">
         <v>127.01326</v>
       </c>
     </row>

</xml_diff>